<commit_message>
Normal maps optimized (RGB8)
</commit_message>
<xml_diff>
--- a/TestConfigurations.xlsx
+++ b/TestConfigurations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Thesis\RSM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016B8EDF-DB8E-4E92-9995-26B3BDA745B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105FBED9-96C0-4A29-A5EB-7593F5C6A675}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1545FC52-C17C-48AF-8A31-F61D7AB71710}"/>
   </bookViews>
@@ -51,12 +51,6 @@
     <t>0.5xApp</t>
   </si>
   <si>
-    <t>1480x720</t>
-  </si>
-  <si>
-    <t>2220x1080</t>
-  </si>
-  <si>
     <t>Scenes</t>
   </si>
   <si>
@@ -187,6 +181,12 @@
   </si>
   <si>
     <t>256x256</t>
+  </si>
+  <si>
+    <t>2220x1080 (Native)</t>
+  </si>
+  <si>
+    <t>1480x720 (HD+)</t>
   </si>
 </sst>
 </file>
@@ -202,12 +202,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -222,8 +240,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CA2B18-38E1-4ABA-B16A-C08F3CEC29BF}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +578,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -566,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -574,24 +595,24 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C2">
         <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>64</v>
@@ -605,7 +626,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -616,7 +637,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -624,31 +645,31 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
         <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>9.15</v>
@@ -662,10 +683,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E10">
         <v>11.3</v>
@@ -673,10 +694,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E11">
         <v>12</v>
@@ -684,9 +705,9 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12">
+        <v>36</v>
+      </c>
+      <c r="C12" s="3">
         <v>29.35</v>
       </c>
       <c r="D12">
@@ -698,10 +719,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E13">
         <v>15.8</v>
@@ -709,7 +730,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E14">
         <v>17</v>
@@ -717,7 +738,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>4.3499999999999996</v>
@@ -731,7 +752,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16">
         <v>3.2</v>
@@ -739,15 +760,15 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17">
+        <v>41</v>
+      </c>
+      <c r="E17" s="2">
         <v>3.1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>14.9</v>
@@ -761,7 +782,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E19">
         <v>8.6</v>
@@ -769,7 +790,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E20">
         <v>8.4</v>
@@ -777,10 +798,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21">
         <v>35.5</v>
@@ -794,7 +815,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E22">
         <v>30</v>
@@ -802,7 +823,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E23">
         <v>30</v>
@@ -810,9 +831,9 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1">
         <v>60</v>
       </c>
       <c r="D24">
@@ -824,7 +845,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E25">
         <v>35</v>
@@ -832,7 +853,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E26">
         <v>35</v>
@@ -840,7 +861,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C27">
         <v>17.8</v>
@@ -854,7 +875,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E28">
         <v>15.7</v>
@@ -862,7 +883,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E29">
         <v>16</v>
@@ -870,7 +891,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C30">
         <v>33.5</v>
@@ -884,7 +905,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E31">
         <v>18.8</v>
@@ -892,7 +913,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E32">
         <v>18.8</v>
@@ -900,24 +921,24 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" t="s">
         <v>31</v>
       </c>
-      <c r="D34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" t="s">
-        <v>33</v>
-      </c>
       <c r="F34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C35">
         <v>6.7</v>
@@ -931,10 +952,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E36">
         <v>11.2</v>
@@ -942,10 +963,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E37">
         <v>12.3</v>
@@ -956,9 +977,9 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38">
+        <v>36</v>
+      </c>
+      <c r="C38" s="3">
         <v>8</v>
       </c>
       <c r="D38">
@@ -970,10 +991,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E39">
         <v>13.8</v>
@@ -981,7 +1002,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E40">
         <v>15.7</v>
@@ -992,9 +1013,9 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41">
+        <v>39</v>
+      </c>
+      <c r="C41" s="2">
         <v>3.4</v>
       </c>
       <c r="D41">
@@ -1006,7 +1027,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E42">
         <v>6.3</v>
@@ -1014,7 +1035,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E43">
         <v>7.3</v>
@@ -1025,7 +1046,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C44">
         <v>4.2</v>
@@ -1039,7 +1060,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E45">
         <v>7.8</v>
@@ -1047,7 +1068,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E46">
         <v>9.1</v>
@@ -1058,10 +1079,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C47">
         <v>14</v>
@@ -1075,7 +1096,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E48">
         <v>24</v>
@@ -1083,7 +1104,7 @@
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E49">
         <v>25.5</v>
@@ -1094,7 +1115,7 @@
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C50">
         <v>15.7</v>
@@ -1108,7 +1129,7 @@
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E51">
         <v>27.5</v>
@@ -1116,18 +1137,18 @@
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E52">
         <v>30</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="1">
         <v>31.2</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C53">
         <v>7.4</v>
@@ -1141,7 +1162,7 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E54">
         <v>14.2</v>
@@ -1149,7 +1170,7 @@
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E55">
         <v>15.3</v>
@@ -1160,7 +1181,7 @@
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C56">
         <v>8.3000000000000007</v>
@@ -1174,7 +1195,7 @@
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E57">
         <v>16.2</v>
@@ -1182,7 +1203,7 @@
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E58">
         <v>17.8</v>

</xml_diff>

<commit_message>
Fixing map precision + Scenes in positive octant
</commit_message>
<xml_diff>
--- a/TestConfigurations.xlsx
+++ b/TestConfigurations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Thesis\RSM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105FBED9-96C0-4A29-A5EB-7593F5C6A675}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83496B83-622C-4ADD-8AE4-3E8C515099BE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1545FC52-C17C-48AF-8A31-F61D7AB71710}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>Indirect Illum Resolution</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Change in settings!</t>
   </si>
   <si>
-    <t>256x256 is not worth!</t>
-  </si>
-  <si>
     <t>262.267 tris</t>
   </si>
   <si>
@@ -187,6 +184,18 @@
   </si>
   <si>
     <t>1480x720 (HD+)</t>
+  </si>
+  <si>
+    <t>Crytek Sponza (pre ASTC)</t>
+  </si>
+  <si>
+    <t>256x256 is worth for Sponza</t>
+  </si>
+  <si>
+    <t>DEFERRED NAIVE FPS</t>
+  </si>
+  <si>
+    <t>DEFERRED INTERPOLATED FPS</t>
   </si>
 </sst>
 </file>
@@ -561,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CA2B18-38E1-4ABA-B16A-C08F3CEC29BF}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +580,7 @@
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="26.140625" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
   </cols>
@@ -598,13 +607,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -612,7 +621,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3">
         <v>64</v>
@@ -658,10 +667,10 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -719,7 +728,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -930,12 +939,12 @@
         <v>31</v>
       </c>
       <c r="F34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
@@ -952,7 +961,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
@@ -963,7 +972,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -991,7 +1000,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>

</xml_diff>